<commit_message>
Added paired comparison to finalconfirmation.xlsx, and Didn't error, so basically added new files, for some reason AIC9 parameters.xlsx changed
</commit_message>
<xml_diff>
--- a/AIC9parameters.xlsx
+++ b/AIC9parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4245ACC0-2F96-4B22-A083-750B583C3B94}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11676468-1A12-4D8E-9A21-07854D3C1985}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{BF1E0B4C-CA9F-48FF-9073-C1300659D61A}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{BF1E0B4C-CA9F-48FF-9073-C1300659D61A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,178 +387,178 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>2204.2292171864119</v>
+        <v>2204.2292170912615</v>
       </c>
       <c r="B1">
-        <v>1385.8249072685196</v>
+        <v>1383.0795960930136</v>
       </c>
       <c r="C1">
-        <v>1434.5268945738233</v>
+        <v>1428.8271839685574</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2227.119236892242</v>
+        <v>2227.1192368807488</v>
       </c>
       <c r="B2">
-        <v>1482.0443111325599</v>
+        <v>1465.9570461612841</v>
       </c>
       <c r="C2">
-        <v>1329.6420308346146</v>
+        <v>1494.2946379747702</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2343.9137069401986</v>
+        <v>2343.9137069530807</v>
       </c>
       <c r="B3">
-        <v>1532.1749237175711</v>
+        <v>1586.5214891726905</v>
       </c>
       <c r="C3">
-        <v>1629.9765789738558</v>
+        <v>1455.6163657279224</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2320.9625294467764</v>
+        <v>2320.962498724236</v>
       </c>
       <c r="B4">
-        <v>1791.2931533693336</v>
+        <v>1774.6466847242061</v>
       </c>
       <c r="C4">
-        <v>1735.3767825141572</v>
+        <v>1705.8701555345397</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2422.653993387893</v>
+        <v>2422.6539933980139</v>
       </c>
       <c r="B5">
-        <v>1663.8644174496033</v>
+        <v>1671.2731630940148</v>
       </c>
       <c r="C5">
-        <v>1642.6288803701384</v>
+        <v>1620.8443032066889</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2360.708546824399</v>
+        <v>2360.7084387163345</v>
       </c>
       <c r="B6">
-        <v>1776.1845810515506</v>
+        <v>1774.6259027478818</v>
       </c>
       <c r="C6">
-        <v>1784.672455274761</v>
+        <v>1784.2650066614551</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1992.9864161741264</v>
+        <v>1992.98484726981</v>
       </c>
       <c r="B7">
-        <v>1556.0413514396798</v>
+        <v>1566.3791362128925</v>
       </c>
       <c r="C7">
-        <v>1533.383976106607</v>
+        <v>1482.5142659959436</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2135.7478413983877</v>
+        <v>2135.7549744213029</v>
       </c>
       <c r="B8">
-        <v>1655.7249330385901</v>
+        <v>1660.8003328907289</v>
       </c>
       <c r="C8">
-        <v>1507.3221427558281</v>
+        <v>1524.1020273468509</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2471.0153725355826</v>
+        <v>2471.0153838041033</v>
       </c>
       <c r="B9">
-        <v>1788.3111565027355</v>
+        <v>1788.3782491419802</v>
       </c>
       <c r="C9">
-        <v>1513.8983550611081</v>
+        <v>1514.0343486951572</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2111.5944047916419</v>
+        <v>2111.5944041864032</v>
       </c>
       <c r="B10">
-        <v>1370.7595654685633</v>
+        <v>1368.6689139450625</v>
       </c>
       <c r="C10">
-        <v>1287.0946321895622</v>
+        <v>1292.6384240066725</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>1970.0041216261243</v>
+        <v>1970.0038839175693</v>
       </c>
       <c r="B11">
-        <v>1414.799188154708</v>
+        <v>1416.2687623358067</v>
       </c>
       <c r="C11">
-        <v>1308.3661889304565</v>
+        <v>1298.5132524254782</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2787.9537177936368</v>
+        <v>2787.9536320270217</v>
       </c>
       <c r="B12">
-        <v>2270.439536824319</v>
+        <v>2270.4512025612389</v>
       </c>
       <c r="C12">
-        <v>2036.7354335933187</v>
+        <v>2036.3897228392641</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2315.1853410977997</v>
+        <v>2315.185341984487</v>
       </c>
       <c r="B13">
-        <v>1763.9087262286291</v>
+        <v>1782.3538751813696</v>
       </c>
       <c r="C13">
-        <v>1803.6382325725028</v>
+        <v>1792.0065844647258</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2593.0481329755003</v>
+        <v>2593.0484738491914</v>
       </c>
       <c r="B14">
-        <v>1922.4486894831293</v>
+        <v>1922.7202893800636</v>
       </c>
       <c r="C14">
-        <v>1703.8062897316559</v>
+        <v>1702.405037810182</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2508.4810606424458</v>
+        <v>2508.6641344546319</v>
       </c>
       <c r="B15">
-        <v>2024.6691965897012</v>
+        <v>2033.5167339667075</v>
       </c>
       <c r="C15">
-        <v>1824.8885139677502</v>
+        <v>1844.9470529650316</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2205.5211166450968</v>
+        <v>2205.5211166450599</v>
       </c>
       <c r="B16">
-        <v>1510.1454648596223</v>
+        <v>1511.4651336237885</v>
       </c>
       <c r="C16">
-        <v>1270.567139051552</v>
+        <v>1268.1754357637358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added input function plot to every plot
</commit_message>
<xml_diff>
--- a/AIC9parameters.xlsx
+++ b/AIC9parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF3999E-2F90-450E-BB0E-F11EF750B491}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F2C1F6-E0DE-43FB-A212-6EF843331A1C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{BF1E0B4C-CA9F-48FF-9073-C1300659D61A}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{BF1E0B4C-CA9F-48FF-9073-C1300659D61A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Added input function plot to every plot"
This reverts commit 11f7516f48c69a4e94eb8b95dbb55ca9f14ed367.
</commit_message>
<xml_diff>
--- a/AIC9parameters.xlsx
+++ b/AIC9parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F2C1F6-E0DE-43FB-A212-6EF843331A1C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF3999E-2F90-450E-BB0E-F11EF750B491}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{BF1E0B4C-CA9F-48FF-9073-C1300659D61A}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{BF1E0B4C-CA9F-48FF-9073-C1300659D61A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Revert "Added input function plot to every plot""
This reverts commit d0bc5392ff0faa2879b404550255126016583cfe.
</commit_message>
<xml_diff>
--- a/AIC9parameters.xlsx
+++ b/AIC9parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF3999E-2F90-450E-BB0E-F11EF750B491}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F2C1F6-E0DE-43FB-A212-6EF843331A1C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{BF1E0B4C-CA9F-48FF-9073-C1300659D61A}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{BF1E0B4C-CA9F-48FF-9073-C1300659D61A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>